<commit_message>
add data service 1.3.0 docu
</commit_message>
<xml_diff>
--- a/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
+++ b/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">17.05.2021 10:32:53</t>
+    <t xml:space="preserve">28.09.2021 18:40:07</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R35a-10</t>
+    <t xml:space="preserve">R35b-03</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -38,12 +38,15 @@
     <t xml:space="preserve">Rückgriff auf veraltete Übersetzungen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexdatei erzeugen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nein</t>
   </si>
   <si>
-    <t xml:space="preserve">Indexdatei erzeugen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Standard-Dateinamen verwenden (ID als Dokumentname)</t>
   </si>
   <si>
@@ -53,9 +56,6 @@
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">Layoutvariante</t>
   </si>
   <si>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">145449190795</t>
+    <t xml:space="preserve">149110787083</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service for Industrial Edge</t>
+    <t xml:space="preserve">Data Service for Industrial Edge V1.3</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">05/2021</t>
+    <t xml:space="preserve">09/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50591892-AB</t>
+    <t xml:space="preserve">A5E50591892-AC</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIABtUsVLi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAAbVLFS4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAASVPFPi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAAElTxT4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -255,31 +255,31 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -295,7 +295,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>145449190795</v>
+        <v>149110787083</v>
       </c>
     </row>
     <row r="20">
@@ -422,7 +422,7 @@
         <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "add 1.4.0 docu"
This reverts commit dcd65d13c5eddd67eb61b91eeeec72f98368abaa.
</commit_message>
<xml_diff>
--- a/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
+++ b/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">11.08.2022 14:46:14</t>
+    <t xml:space="preserve">28.09.2021 18:40:07</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R37b-04</t>
+    <t xml:space="preserve">R35b-03</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">Produktionssprache</t>
   </si>
   <si>
-    <t xml:space="preserve">de-DE, en-US, zh-CHS, es-ES</t>
+    <t xml:space="preserve">de-DE, en-US</t>
   </si>
   <si>
     <t xml:space="preserve">Warnhinweis-Layout</t>
@@ -38,21 +38,21 @@
     <t xml:space="preserve">Rückgriff auf veraltete Übersetzungen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexdatei erzeugen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nein</t>
   </si>
   <si>
-    <t xml:space="preserve">Indexdatei erzeugen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Standard-Dateinamen verwenden (ID als Dokumentname)</t>
   </si>
   <si>
     <t xml:space="preserve">IDs an Topic-Titel anfügen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">159517802123</t>
+    <t xml:space="preserve">149110787083</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service for Industrial Edge V1.4</t>
+    <t xml:space="preserve">Data Service for Industrial Edge V1.3</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,13 +107,13 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">08/2022; V1.4</t>
+    <t xml:space="preserve">09/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 - 2022</t>
+    <t xml:space="preserve">2021</t>
   </si>
   <si>
     <t xml:space="preserve">Dokument-Bestellnummer</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50591892-AD</t>
+    <t xml:space="preserve">A5E50591892-AC</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIAMd1C1Xi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACADHdQtV4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAASVPFPi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAAElTxT4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -255,23 +255,23 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -279,7 +279,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -295,7 +295,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>159517802123</v>
+        <v>149110787083</v>
       </c>
     </row>
     <row r="20">
@@ -422,7 +422,7 @@
         <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Service 1.6.0 release
</commit_message>
<xml_diff>
--- a/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
+++ b/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">21.10.2022 10:25:00</t>
+    <t xml:space="preserve">24.02.2023 11:05:59</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R37b-04</t>
+    <t xml:space="preserve">R38b-04</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">Produktionssprache</t>
   </si>
   <si>
-    <t xml:space="preserve">de-DE, en-US, es-ES, zh-CHS</t>
+    <t xml:space="preserve">de-DE, en-US, fr-FR, it-IT, es-ES, zh-CHS</t>
   </si>
   <si>
     <t xml:space="preserve">Warnhinweis-Layout</t>
@@ -50,12 +50,12 @@
     <t xml:space="preserve">IDs an Topic-Titel anfügen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">Layoutvariante</t>
   </si>
   <si>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">161694842635</t>
+    <t xml:space="preserve">165621632779</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service for Industrial Edge V1.5</t>
+    <t xml:space="preserve">Data Service for Industrial Edge V1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,13 +107,13 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">10/2022; V1.5</t>
+    <t xml:space="preserve">02/2023; V1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 - 2022</t>
+    <t xml:space="preserve">2021 - 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Dokument-Bestellnummer</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50591892-AE</t>
+    <t xml:space="preserve">A5E50591892-AF</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIACBTVVXi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAAgU1VV4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAL1YWFbi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAC9WFhW4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -271,15 +271,15 @@
         <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>161694842635</v>
+        <v>165621632779</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
Release 1 6 (#11)
* Data Service 1.6.0 release

* fix comment

* add missing files

* add 1.6.0 devkit docu

* Update README-dataservicedevelopmentkit.md

* Update README-dataservicesimulation.md

---------

Co-authored-by: Norman Hummel <74044913+HummelN7872@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
+++ b/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">21.10.2022 10:25:00</t>
+    <t xml:space="preserve">24.02.2023 11:05:59</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R37b-04</t>
+    <t xml:space="preserve">R38b-04</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">Produktionssprache</t>
   </si>
   <si>
-    <t xml:space="preserve">de-DE, en-US, es-ES, zh-CHS</t>
+    <t xml:space="preserve">de-DE, en-US, fr-FR, it-IT, es-ES, zh-CHS</t>
   </si>
   <si>
     <t xml:space="preserve">Warnhinweis-Layout</t>
@@ -50,12 +50,12 @@
     <t xml:space="preserve">IDs an Topic-Titel anfügen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">Layoutvariante</t>
   </si>
   <si>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">161694842635</t>
+    <t xml:space="preserve">165621632779</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service for Industrial Edge V1.5</t>
+    <t xml:space="preserve">Data Service for Industrial Edge V1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,13 +107,13 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">10/2022; V1.5</t>
+    <t xml:space="preserve">02/2023; V1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
   </si>
   <si>
-    <t xml:space="preserve">2021 - 2022</t>
+    <t xml:space="preserve">2021 - 2023</t>
   </si>
   <si>
     <t xml:space="preserve">Dokument-Bestellnummer</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50591892-AE</t>
+    <t xml:space="preserve">A5E50591892-AF</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIACBTVVXi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAAgU1VV4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAL1YWFbi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAC9WFhW4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -271,15 +271,15 @@
         <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>161694842635</v>
+        <v>165621632779</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
release of Data Service 1.7.0
</commit_message>
<xml_diff>
--- a/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
+++ b/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">24.02.2023 11:05:59</t>
+    <t xml:space="preserve">31.05.2023 11:46:31</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R38b-04</t>
+    <t xml:space="preserve">R38c-03</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -38,21 +38,21 @@
     <t xml:space="preserve">Rückgriff auf veraltete Übersetzungen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexdatei erzeugen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nein</t>
   </si>
   <si>
-    <t xml:space="preserve">Indexdatei erzeugen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Standard-Dateinamen verwenden (ID als Dokumentname)</t>
   </si>
   <si>
     <t xml:space="preserve">IDs an Topic-Titel anfügen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">165621632779</t>
+    <t xml:space="preserve">169127091979</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service for Industrial Edge V1.6</t>
+    <t xml:space="preserve">Data Service for Industrial Edge V1.7</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">02/2023; V1.6</t>
+    <t xml:space="preserve">05/2023; V1.7</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50591892-AF</t>
+    <t xml:space="preserve">A5E50591892-AG</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIAL1YWFbi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAC9WFhW4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAM9dv1bi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACADPXb9W4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -255,23 +255,23 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -279,7 +279,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -295,7 +295,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>165621632779</v>
+        <v>169127091979</v>
       </c>
     </row>
     <row r="20">
@@ -422,7 +422,7 @@
         <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
release of Data Service 1.7.0 (#13)
* release of Data Service 1.7.0

* Update and rename docker-compose.yml to docker-compose.example.yml

* Update README.md

Added hint for renaming the docker-compose file

* Update README.md

* Update README-dataservicedevelopmentkit.md

Added 1.7.0 tag to dockerhub description

---------

Co-authored-by: Norman Hummel <74044913+HummelN7872@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
+++ b/docs/data-service/html5-documentation-data-service/ProductionSummary.xlsx
@@ -8,13 +8,13 @@
     <t xml:space="preserve">Produktionszeitpunkt</t>
   </si>
   <si>
-    <t xml:space="preserve">24.02.2023 11:05:59</t>
+    <t xml:space="preserve">31.05.2023 11:46:31</t>
   </si>
   <si>
     <t xml:space="preserve">Systeminformation</t>
   </si>
   <si>
-    <t xml:space="preserve">R38b-04</t>
+    <t xml:space="preserve">R38c-03</t>
   </si>
   <si>
     <t xml:space="preserve">Produktion</t>
@@ -38,21 +38,21 @@
     <t xml:space="preserve">Rückgriff auf veraltete Übersetzungen</t>
   </si>
   <si>
+    <t xml:space="preserve">Ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexdatei erzeugen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nein</t>
   </si>
   <si>
-    <t xml:space="preserve">Indexdatei erzeugen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Standard-Dateinamen verwenden (ID als Dokumentname)</t>
   </si>
   <si>
     <t xml:space="preserve">IDs an Topic-Titel anfügen</t>
   </si>
   <si>
-    <t xml:space="preserve">Ja</t>
-  </si>
-  <si>
     <t xml:space="preserve">Temporäre Dateien löschen</t>
   </si>
   <si>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">Knoten-ID</t>
   </si>
   <si>
-    <t xml:space="preserve">165621632779</t>
+    <t xml:space="preserve">169127091979</t>
   </si>
   <si>
     <t xml:space="preserve">Titel</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Service for Industrial Edge V1.6</t>
+    <t xml:space="preserve">Data Service for Industrial Edge V1.7</t>
   </si>
   <si>
     <t xml:space="preserve">Dateiname</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">Ausgabestand</t>
   </si>
   <si>
-    <t xml:space="preserve">02/2023; V1.6</t>
+    <t xml:space="preserve">05/2023; V1.7</t>
   </si>
   <si>
     <t xml:space="preserve">Copyright-Jahreszahlen</t>
@@ -122,7 +122,7 @@
     <t xml:space="preserve">Dokument-Identifikationsnummer</t>
   </si>
   <si>
-    <t xml:space="preserve">A5E50591892-AF</t>
+    <t xml:space="preserve">A5E50591892-AG</t>
   </si>
   <si>
     <t xml:space="preserve">Innentitel-Infofeld</t>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">PDF verlinken</t>
   </si>
   <si>
-    <t xml:space="preserve">UEsDBBQAAAAIAL1YWFbi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACAC9WFhW4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
+    <t xml:space="preserve">UEsDBBQAAAAIAM9dv1bi/LD+YAAAAGsAAAALAAAAc3lzRGF0YS54bWx7v3u/jX1Fbo5CWWpRcWZ+nq2SoZ6BkkJqXnJ+SmZeuq1SaUmaroWSQnFJYl5KYk5+XqqtUmVqsZK9nU1KYkkisjZDoE49Y3NDSyU7m4Ki/ILUopLM1GIFfTsbfZBSOwBQSwECFAAUAAAACADPXb9W4vyw/mAAAABrAAAACwAAAAAAAAAAAAAAAAAAAAAAc3lzRGF0YS54bWxQSwUGAAAAAAEAAQA5AAAAiQAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -255,23 +255,23 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -279,7 +279,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -295,7 +295,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
@@ -332,7 +332,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>165621632779</v>
+        <v>169127091979</v>
       </c>
     </row>
     <row r="20">
@@ -422,7 +422,7 @@
         <v>45</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>